<commit_message>
add find outliers for analyzing excel file
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work2\githubs\DataStat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B86185A-ACD1-4154-84A6-98EDFD8A1F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70900DC8-F775-418B-B3A8-5D4F007E5522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>CeLiang-A</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -35,11 +35,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CeLiang-D</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>美丽</t>
+    <t>CeLiang-C</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -365,20 +361,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C2" sqref="C2:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="12.1484375" customWidth="1"/>
-    <col min="2" max="3" width="10.69921875" customWidth="1"/>
-    <col min="4" max="4" width="10.546875" customWidth="1"/>
+    <col min="1" max="12" width="12.1484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -386,385 +380,285 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>10.0999</v>
       </c>
       <c r="B2">
-        <v>6.0004799999999996</v>
+        <v>6.1987199999999998</v>
       </c>
       <c r="C2">
-        <v>5.6992500000000001</v>
-      </c>
-      <c r="D2">
-        <v>14.500400000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+        <v>17.223400000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>9.9565199999999994</v>
       </c>
       <c r="B3">
-        <v>5.9577799999999996</v>
+        <v>4.4782799999999998</v>
       </c>
       <c r="C3">
-        <v>4.6956600000000002</v>
-      </c>
-      <c r="D3">
-        <v>14.817600000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+        <v>21.534800000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>10.078200000000001</v>
       </c>
       <c r="B4">
-        <v>6.1540499999999998</v>
+        <v>11</v>
       </c>
       <c r="C4">
-        <v>5.5472599999999996</v>
-      </c>
-      <c r="D4">
-        <v>16.8443</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+        <v>18.527899999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>9.9969900000000003</v>
       </c>
       <c r="B5">
-        <v>6.0094700000000003</v>
+        <v>5.9381599999999999</v>
       </c>
       <c r="C5">
-        <v>4.9789599999999998</v>
-      </c>
-      <c r="D5">
-        <v>14.757199999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+        <v>21.159400000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>10.0824</v>
       </c>
       <c r="B6">
-        <v>6.1524700000000001</v>
+        <v>4.96394</v>
       </c>
       <c r="C6">
-        <v>5.5769799999999998</v>
-      </c>
-      <c r="D6">
-        <v>16.9969</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
+        <v>19.235700000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>9.9943299999999997</v>
       </c>
       <c r="B7">
-        <v>6.1216799999999996</v>
+        <v>5.9891199999999998</v>
       </c>
       <c r="C7">
-        <v>4.9603000000000002</v>
-      </c>
-      <c r="D7">
-        <v>15.004799999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
+        <v>24.1218</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>9.90991</v>
       </c>
       <c r="B8">
-        <v>5.98637</v>
+        <v>4.93194</v>
       </c>
       <c r="C8">
-        <v>4.3693900000000001</v>
-      </c>
-      <c r="D8">
-        <v>14.5778</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+        <v>17.5304</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A9">
         <v>9.9925300000000004</v>
       </c>
       <c r="B9">
-        <v>5.9800800000000001</v>
+        <v>3.9189500000000002</v>
       </c>
       <c r="C9">
-        <v>4.9477099999999998</v>
-      </c>
-      <c r="D9">
-        <v>16.540500000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+        <v>22.3307</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A10">
         <v>10.0008</v>
       </c>
       <c r="B10">
-        <v>5.9706200000000003</v>
+        <v>4.9103500000000002</v>
       </c>
       <c r="C10">
-        <v>5.0055399999999999</v>
-      </c>
-      <c r="D10">
-        <v>15.0947</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
+        <v>19.0916</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A11">
         <v>9.9589200000000009</v>
       </c>
       <c r="B11">
-        <v>5.9881599999999997</v>
+        <v>5.0094900000000004</v>
       </c>
       <c r="C11">
-        <v>4.7124699999999997</v>
-      </c>
-      <c r="D11">
-        <v>16.524699999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.5">
+        <v>19.730499999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A12">
         <v>10.139099999999999</v>
       </c>
       <c r="B12">
-        <v>5.8839699999999997</v>
+        <v>4.5070800000000002</v>
       </c>
       <c r="C12">
-        <v>5.97384</v>
-      </c>
-      <c r="D12">
-        <v>16.216799999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.5">
+        <v>19.000699999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A13">
         <v>9.9014900000000008</v>
       </c>
       <c r="B13">
-        <v>6.0012400000000001</v>
+        <v>6.6694300000000002</v>
       </c>
       <c r="C13">
-        <v>4.3104500000000003</v>
-      </c>
-      <c r="D13">
-        <v>14.8637</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.5">
+        <v>19.635100000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>3.81792</v>
+      </c>
+      <c r="C14">
+        <v>23.688600000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A15">
         <v>9.9951100000000004</v>
       </c>
-      <c r="B14">
-        <v>6.0022099999999998</v>
-      </c>
-      <c r="C14">
-        <v>4.9657400000000003</v>
-      </c>
-      <c r="D14">
-        <v>14.800800000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A15">
+      <c r="B15">
+        <v>4.9412700000000003</v>
+      </c>
+      <c r="C15">
+        <v>19.514299999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A16">
         <v>9.8556699999999999</v>
       </c>
-      <c r="B15">
-        <v>5.9928699999999999</v>
-      </c>
-      <c r="C15">
-        <v>3.9896699999999998</v>
-      </c>
-      <c r="D15">
-        <v>14.706200000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A16">
+      <c r="B16">
+        <v>3.2679999999999998</v>
+      </c>
+      <c r="C16">
+        <v>23.9937</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A17">
         <v>9.8939299999999992</v>
       </c>
-      <c r="B16">
-        <v>5.8678400000000002</v>
-      </c>
-      <c r="C16">
-        <v>4.25753</v>
-      </c>
-      <c r="D16">
-        <v>14.881600000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A17">
+      <c r="B17">
+        <v>3.7271999999999998</v>
+      </c>
+      <c r="C17">
+        <v>20.009599999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A18">
         <v>9.8611699999999995</v>
       </c>
-      <c r="B17">
-        <v>6.1744300000000001</v>
-      </c>
-      <c r="C17">
-        <v>4.0281900000000004</v>
-      </c>
-      <c r="D17">
-        <v>13.839700000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A18">
+      <c r="C18">
+        <v>19.1556</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A19">
         <v>10.076700000000001</v>
       </c>
-      <c r="B18">
-        <v>5.9667599999999998</v>
-      </c>
-      <c r="C18">
-        <v>5.5371800000000002</v>
-      </c>
-      <c r="D18">
-        <v>15.0124</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A19">
+      <c r="C19">
+        <v>23.081099999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A20">
         <v>9.9263999999999992</v>
       </c>
-      <c r="B19">
-        <v>5.9752700000000001</v>
-      </c>
-      <c r="C19">
-        <v>4.4847799999999998</v>
-      </c>
-      <c r="D19">
-        <v>15.0221</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A20">
+      <c r="C20">
+        <v>20.189499999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A21">
         <v>10.058</v>
       </c>
-      <c r="B20">
-        <v>5.8819800000000004</v>
-      </c>
-      <c r="C20">
-        <v>5.4058000000000002</v>
-      </c>
-      <c r="D20">
-        <v>14.928699999999999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A21">
+      <c r="C21">
+        <v>23.049399999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A22">
         <v>9.9617900000000006</v>
       </c>
-      <c r="B21">
-        <v>5.88096</v>
-      </c>
-      <c r="C21">
-        <v>4.7325100000000004</v>
-      </c>
-      <c r="D21">
-        <v>13.6784</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A22">
+      <c r="C22">
+        <v>22.433499999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A23">
         <v>10.206099999999999</v>
       </c>
-      <c r="B22">
-        <v>5.7990199999999996</v>
-      </c>
-      <c r="C22">
-        <v>6.4426300000000003</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A23">
+      <c r="C23">
+        <v>19.727399999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A24">
         <v>9.8765199999999993</v>
       </c>
-      <c r="B23">
-        <v>6.1338400000000002</v>
-      </c>
-      <c r="C23">
-        <v>4.1356299999999999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A24">
+      <c r="C24">
+        <v>19.601600000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A25">
         <v>10.1165</v>
       </c>
-      <c r="B24">
-        <v>6.0488200000000001</v>
-      </c>
-      <c r="C24">
-        <v>5.8157399999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A25">
+      <c r="C25">
+        <v>19.412500000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A26">
         <v>9.95458</v>
       </c>
-      <c r="B25">
-        <v>6.0296399999999997</v>
-      </c>
-      <c r="C25">
-        <v>4.6820599999999999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A26">
+      <c r="C26">
+        <v>19.763300000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A27">
         <v>9.9865200000000005</v>
       </c>
-      <c r="B26">
-        <v>6.0243900000000004</v>
-      </c>
-      <c r="C26">
-        <v>4.9056600000000001</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A27">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A28">
         <v>9.9500399999999996</v>
       </c>
-      <c r="B27">
-        <v>5.8907699999999998</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A28">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A29">
         <v>9.9817599999999995</v>
       </c>
-      <c r="B28">
-        <v>5.9400899999999996</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A29">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A30">
         <v>10.1844</v>
       </c>
-      <c r="B29">
-        <v>5.9212100000000003</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A30">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A31">
         <v>9.9757200000000008</v>
       </c>
-      <c r="B30">
-        <v>5.7419900000000004</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A31">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A32">
         <v>10.1997</v>
-      </c>
-      <c r="B31">
-        <v>5.8783500000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>